<commit_message>
Update home page and edit personal details tests
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -5,21 +5,21 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etabib\workspace\Auto_CQM\src\com\generic\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\git\callawaygolf1\src\com\generic\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="8970" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="8970" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
     <sheet name="SetupRunners" sheetId="43" r:id="rId2"/>
     <sheet name="PersonalDetailsRegression" sheetId="50" r:id="rId3"/>
     <sheet name="EmailAddressRegression" sheetId="51" r:id="rId4"/>
-    <sheet name="HomePageRegression" sheetId="46" r:id="rId5"/>
-    <sheet name="RegistrationRegression" sheetId="24" r:id="rId6"/>
-    <sheet name="LoginRegression" sheetId="41" r:id="rId7"/>
-    <sheet name="PasswordRegression" sheetId="47" r:id="rId8"/>
+    <sheet name="PasswordRegression" sheetId="47" r:id="rId5"/>
+    <sheet name="HomePageRegression" sheetId="46" r:id="rId6"/>
+    <sheet name="RegistrationRegression" sheetId="24" r:id="rId7"/>
+    <sheet name="LoginRegression" sheetId="41" r:id="rId8"/>
     <sheet name="AccountSetup" sheetId="37" r:id="rId9"/>
     <sheet name="users" sheetId="13" r:id="rId10"/>
     <sheet name="products" sheetId="8" r:id="rId11"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="443">
   <si>
     <t>Browser</t>
   </si>
@@ -1172,13 +1172,6 @@
     <t>Personal Details Without firstName and lastName</t>
   </si>
   <si>
-    <t>Original Personal Details</t>
-  </si>
-  <si>
-    <t>click update 
-revert changes</t>
-  </si>
-  <si>
     <t>The email you entered is not available</t>
   </si>
   <si>
@@ -1335,9 +1328,6 @@
     <t>PD-06</t>
   </si>
   <si>
-    <t>PD-07</t>
-  </si>
-  <si>
     <t>A6</t>
   </si>
   <si>
@@ -1393,18 +1383,35 @@
   </si>
   <si>
     <t>confirmNewPasswordErrors:Password does not meet minimum requirements.</t>
+  </si>
+  <si>
+    <t>update Personal Details</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1612,27 +1619,27 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1641,7 +1648,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1653,17 +1660,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1672,7 +1679,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1687,26 +1694,26 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1718,10 +1725,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1736,16 +1743,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1755,7 +1762,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1767,7 +1774,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1776,18 +1783,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1796,78 +1803,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2247,7 +2258,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3478,13 +3489,13 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B7" s="64" t="s">
-        <v>427</v>
-      </c>
-      <c r="C7" s="93" t="s">
-        <v>428</v>
+        <v>424</v>
+      </c>
+      <c r="C7" s="92" t="s">
+        <v>425</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>272</v>
@@ -3493,14 +3504,14 @@
         <v>271</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>268</v>
@@ -3779,10 +3790,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3834,7 +3845,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="90" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B2" s="70" t="s">
         <v>7</v>
@@ -3845,8 +3856,8 @@
       <c r="D2" s="71" t="s">
         <v>360</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>31</v>
+      <c r="E2" s="95" t="s">
+        <v>102</v>
       </c>
       <c r="F2" s="89" t="s">
         <v>355</v>
@@ -3860,7 +3871,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="90" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B3" s="70" t="s">
         <v>7</v>
@@ -3871,8 +3882,8 @@
       <c r="D3" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>31</v>
+      <c r="E3" s="95" t="s">
+        <v>107</v>
       </c>
       <c r="F3" s="71" t="s">
         <v>362</v>
@@ -3886,19 +3897,19 @@
     </row>
     <row r="4" spans="1:10" ht="30">
       <c r="A4" s="90" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B4" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="71" t="s">
-        <v>361</v>
+      <c r="C4" s="96" t="s">
+        <v>442</v>
       </c>
       <c r="D4" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>31</v>
+      <c r="E4" s="95" t="s">
+        <v>111</v>
       </c>
       <c r="F4" s="71" t="s">
         <v>362</v>
@@ -3914,7 +3925,7 @@
     </row>
     <row r="5" spans="1:10" ht="30">
       <c r="A5" s="90" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B5" s="70" t="s">
         <v>7</v>
@@ -3925,8 +3936,8 @@
       <c r="D5" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>31</v>
+      <c r="E5" s="95" t="s">
+        <v>115</v>
       </c>
       <c r="F5" s="71"/>
       <c r="G5" s="71" t="s">
@@ -3942,7 +3953,7 @@
     </row>
     <row r="6" spans="1:10" ht="30">
       <c r="A6" s="90" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B6" s="70" t="s">
         <v>7</v>
@@ -3953,8 +3964,8 @@
       <c r="D6" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>31</v>
+      <c r="E6" s="95" t="s">
+        <v>58</v>
       </c>
       <c r="F6" s="71" t="s">
         <v>362</v>
@@ -3970,7 +3981,7 @@
     </row>
     <row r="7" spans="1:10" ht="30">
       <c r="A7" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B7" s="70" t="s">
         <v>7</v>
@@ -3981,8 +3992,8 @@
       <c r="D7" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>31</v>
+      <c r="E7" s="95" t="s">
+        <v>59</v>
       </c>
       <c r="F7" s="71"/>
       <c r="G7" s="71"/>
@@ -3995,34 +4006,6 @@
       <c r="J7" s="72" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="30">
-      <c r="A8" s="90" t="s">
-        <v>425</v>
-      </c>
-      <c r="B8" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="71" t="s">
-        <v>371</v>
-      </c>
-      <c r="D8" s="71" t="s">
-        <v>372</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="89" t="s">
-        <v>355</v>
-      </c>
-      <c r="G8" s="89" t="s">
-        <v>186</v>
-      </c>
-      <c r="H8" s="73" t="s">
-        <v>364</v>
-      </c>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4073,10 +4056,10 @@
         <v>25</v>
       </c>
       <c r="F1" s="88" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G1" s="88" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H1" s="88" t="s">
         <v>65</v>
@@ -4085,30 +4068,30 @@
         <v>53</v>
       </c>
       <c r="J1" s="86" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="K1" s="85" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L1" s="85" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="81" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B2" s="81" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="79" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D2" s="91" t="s">
         <v>360</v>
       </c>
-      <c r="E2" s="92" t="s">
-        <v>31</v>
+      <c r="E2" s="94" t="s">
+        <v>29</v>
       </c>
       <c r="F2" s="71"/>
       <c r="G2" s="71"/>
@@ -4120,25 +4103,25 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="81" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B3" s="81" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D3" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="92" t="s">
-        <v>33</v>
+      <c r="E3" s="94" t="s">
+        <v>63</v>
       </c>
       <c r="F3" s="84" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G3" s="84" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H3" s="79">
         <v>1234567</v>
@@ -4150,25 +4133,25 @@
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" s="81" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B4" s="81" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D4" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="92" t="s">
-        <v>34</v>
+      <c r="E4" s="94" t="s">
+        <v>64</v>
       </c>
       <c r="F4" s="82" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G4" s="82" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H4" s="79">
         <v>1234567</v>
@@ -4182,23 +4165,23 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="81" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B5" s="81" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D5" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="E5" s="92" t="s">
-        <v>35</v>
+      <c r="E5" s="94" t="s">
+        <v>149</v>
       </c>
       <c r="F5" s="71"/>
       <c r="G5" s="80" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H5" s="79">
         <v>1234567</v>
@@ -4214,22 +4197,22 @@
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" s="81" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B6" s="81" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D6" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="92" t="s">
-        <v>36</v>
+      <c r="E6" s="94" t="s">
+        <v>80</v>
       </c>
       <c r="F6" s="82" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="G6" s="71"/>
       <c r="H6" s="79">
@@ -4240,31 +4223,31 @@
       </c>
       <c r="J6" s="78"/>
       <c r="K6" s="78" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L6" s="77"/>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" s="81" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B7" s="81" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D7" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="92" t="s">
-        <v>37</v>
+      <c r="E7" s="94" t="s">
+        <v>84</v>
       </c>
       <c r="F7" s="80" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G7" s="80" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H7" s="79"/>
       <c r="I7" s="78" t="s">
@@ -4273,30 +4256,30 @@
       <c r="J7" s="78"/>
       <c r="K7" s="78"/>
       <c r="L7" s="77" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="81" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B8" s="81" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="79" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D8" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="E8" s="92" t="s">
-        <v>38</v>
+      <c r="E8" s="94" t="s">
+        <v>88</v>
       </c>
       <c r="F8" s="71" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G8" s="80" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H8" s="79">
         <v>1234567</v>
@@ -4312,25 +4295,25 @@
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" s="81" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B9" s="81" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="79" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D9" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="E9" s="92" t="s">
-        <v>31</v>
+      <c r="E9" s="94" t="s">
+        <v>29</v>
       </c>
       <c r="F9" s="80" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G9" s="71" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H9" s="79">
         <v>1234567</v>
@@ -4340,31 +4323,31 @@
       </c>
       <c r="J9" s="78"/>
       <c r="K9" s="78" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L9" s="77"/>
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" s="81" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B10" s="81" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D10" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="E10" s="92" t="s">
-        <v>33</v>
+      <c r="E10" s="94" t="s">
+        <v>63</v>
       </c>
       <c r="F10" s="80" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G10" s="80" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H10" s="79">
         <v>1234567</v>
@@ -4374,31 +4357,31 @@
       </c>
       <c r="J10" s="78"/>
       <c r="K10" s="78" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L10" s="77"/>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="81" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B11" s="81" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="79" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D11" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="92" t="s">
-        <v>34</v>
+      <c r="E11" s="94" t="s">
+        <v>64</v>
       </c>
       <c r="F11" s="80" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G11" s="80" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H11" s="79">
         <v>874531324</v>
@@ -4409,30 +4392,30 @@
       <c r="J11" s="78"/>
       <c r="K11" s="78"/>
       <c r="L11" s="77" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="81" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B12" s="81" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D12" s="71" t="s">
-        <v>375</v>
-      </c>
-      <c r="E12" s="92" t="s">
-        <v>35</v>
+        <v>373</v>
+      </c>
+      <c r="E12" s="94" t="s">
+        <v>149</v>
       </c>
       <c r="F12" s="80" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G12" s="80" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H12" s="79">
         <v>1234567</v>
@@ -4441,7 +4424,7 @@
         <v>366</v>
       </c>
       <c r="J12" s="78" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="K12" s="78"/>
       <c r="L12" s="77"/>
@@ -4457,610 +4440,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="9.140625" style="51"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="50" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="45">
-      <c r="A2" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="53" t="s">
-        <v>317</v>
-      </c>
-      <c r="D2" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="53" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="45">
-      <c r="A3" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="53" t="s">
-        <v>315</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>314</v>
-      </c>
-      <c r="E3" s="53" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45">
-      <c r="A4" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="53" t="s">
-        <v>318</v>
-      </c>
-      <c r="D4" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="53" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45">
-      <c r="A5" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="53" t="s">
-        <v>319</v>
-      </c>
-      <c r="D5" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="53" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45">
-      <c r="A6" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="53" t="s">
-        <v>317</v>
-      </c>
-      <c r="D6" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="53" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45">
-      <c r="A7" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="53" t="s">
-        <v>315</v>
-      </c>
-      <c r="D7" s="53" t="s">
-        <v>316</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45">
-      <c r="A8" s="53" t="s">
-        <v>323</v>
-      </c>
-      <c r="B8" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="53" t="s">
-        <v>318</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45">
-      <c r="A9" s="53" t="s">
-        <v>324</v>
-      </c>
-      <c r="B9" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="53" t="s">
-        <v>319</v>
-      </c>
-      <c r="D9" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="53" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="53" t="s">
-        <v>351</v>
-      </c>
-      <c r="B10" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="53" t="s">
-        <v>350</v>
-      </c>
-      <c r="D10" s="53" t="s">
-        <v>353</v>
-      </c>
-      <c r="E10" s="53"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="53" t="s">
-        <v>352</v>
-      </c>
-      <c r="B11" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="66" t="s">
-        <v>349</v>
-      </c>
-      <c r="D11" s="66" t="s">
-        <v>354</v>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="8" tint="-0.499984740745262"/>
-  </sheetPr>
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="9.140625" style="39"/>
-    <col min="3" max="3" width="45.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71" style="17" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="17"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="39" customFormat="1">
-      <c r="A1" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="39" customFormat="1">
-      <c r="A2" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="40" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="39" customFormat="1">
-      <c r="A3" s="47" t="s">
-        <v>347</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>346</v>
-      </c>
-      <c r="D3" s="49" t="s">
-        <v>348</v>
-      </c>
-      <c r="E3" s="40" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="40" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="150">
-      <c r="A5" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="61" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="40" t="s">
-        <v>311</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="8" tint="-0.499984740745262"/>
-  </sheetPr>
-  <dimension ref="A1:F14"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="9.140625" style="39"/>
-    <col min="3" max="3" width="33.28515625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="6" style="17" customWidth="1"/>
-    <col min="6" max="6" width="69.42578125" style="17" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="17"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="39" customFormat="1">
-      <c r="A1" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="41"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="44" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A5" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="44" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="44" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30">
-      <c r="A7" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="44" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>101</v>
-      </c>
-      <c r="D8" s="44" t="s">
-        <v>101</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="44" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>328</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>328</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="44"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="22" t="s">
-        <v>337</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>329</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>329</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="44"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="22" t="s">
-        <v>338</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="62" t="s">
-        <v>333</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>332</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="44"/>
-    </row>
-    <row r="12" spans="1:6" ht="30">
-      <c r="A12" s="22" t="s">
-        <v>339</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>330</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>331</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="41"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="22" t="s">
-        <v>340</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="63" t="s">
-        <v>334</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="22" t="s">
-        <v>341</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="63" t="s">
-        <v>335</v>
-      </c>
-      <c r="D14" s="63" t="s">
-        <v>335</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="8" tint="-0.499984740745262"/>
-  </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5103,7 +4486,7 @@
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>7</v>
@@ -5127,7 +4510,7 @@
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>7</v>
@@ -5153,7 +4536,7 @@
     </row>
     <row r="4" spans="1:8" ht="30">
       <c r="A4" s="34" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>7</v>
@@ -5179,7 +4562,7 @@
     </row>
     <row r="5" spans="1:8" ht="60">
       <c r="A5" s="34" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>7</v>
@@ -5205,7 +4588,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="34" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>7</v>
@@ -5224,12 +4607,12 @@
         <v>108</v>
       </c>
       <c r="H6" s="38" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
       <c r="A7" s="34" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>7</v>
@@ -5255,7 +4638,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="34" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>7</v>
@@ -5274,12 +4657,12 @@
       </c>
       <c r="G8" s="34"/>
       <c r="H8" s="38" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
       <c r="A9" s="34" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>7</v>
@@ -5305,7 +4688,7 @@
     </row>
     <row r="10" spans="1:8" ht="30">
       <c r="A10" s="34" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>7</v>
@@ -5331,7 +4714,7 @@
     </row>
     <row r="11" spans="1:8" ht="30">
       <c r="A11" s="34" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>7</v>
@@ -5358,6 +4741,608 @@
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="51"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45">
+      <c r="A2" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="65"/>
+      <c r="C2" s="53" t="s">
+        <v>317</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="53" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45">
+      <c r="A3" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="65"/>
+      <c r="C3" s="53" t="s">
+        <v>315</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>314</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45">
+      <c r="A4" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="65"/>
+      <c r="C4" s="53" t="s">
+        <v>318</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45">
+      <c r="A5" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="65"/>
+      <c r="C5" s="53" t="s">
+        <v>319</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45">
+      <c r="A6" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>317</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45">
+      <c r="A7" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>315</v>
+      </c>
+      <c r="D7" s="53" t="s">
+        <v>316</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45">
+      <c r="A8" s="53" t="s">
+        <v>323</v>
+      </c>
+      <c r="B8" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45">
+      <c r="A9" s="53" t="s">
+        <v>324</v>
+      </c>
+      <c r="B9" s="65"/>
+      <c r="C9" s="53" t="s">
+        <v>319</v>
+      </c>
+      <c r="D9" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="53" t="s">
+        <v>351</v>
+      </c>
+      <c r="B10" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>350</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>353</v>
+      </c>
+      <c r="E10" s="53"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="53" t="s">
+        <v>352</v>
+      </c>
+      <c r="B11" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>349</v>
+      </c>
+      <c r="D11" s="66" t="s">
+        <v>354</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D2:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="39"/>
+    <col min="3" max="3" width="45.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71" style="17" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="39" customFormat="1">
+      <c r="A1" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="39" customFormat="1">
+      <c r="A2" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="39" customFormat="1">
+      <c r="A3" s="47" t="s">
+        <v>347</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>346</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>348</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="150">
+      <c r="A5" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>311</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="39"/>
+    <col min="3" max="3" width="33.28515625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="6" style="17" customWidth="1"/>
+    <col min="6" max="6" width="69.42578125" style="17" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="39" customFormat="1">
+      <c r="A1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="41"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A5" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="41"/>
+      <c r="F6" s="44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30">
+      <c r="A7" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="44" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>328</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>328</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="44"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>329</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>329</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="44"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="62" t="s">
+        <v>333</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="44"/>
+    </row>
+    <row r="12" spans="1:6" ht="30">
+      <c r="A12" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>330</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>331</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="41"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>334</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="63" t="s">
+        <v>335</v>
+      </c>
+      <c r="D14" s="63" t="s">
+        <v>335</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5368,8 +5353,8 @@
   </sheetPr>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5412,7 +5397,7 @@
         <v>24</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>25</v>
@@ -5422,7 +5407,9 @@
       <c r="A2" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="B2" s="23"/>
+      <c r="B2" s="23" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="24" t="s">
         <v>56</v>
       </c>
@@ -5436,7 +5423,7 @@
         <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>28</v>
@@ -5452,7 +5439,9 @@
       <c r="A3" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="23" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="24" t="s">
         <v>56</v>
       </c>
@@ -5466,12 +5455,12 @@
         <v>30</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="94">
+      <c r="I3" s="93">
         <v>0</v>
       </c>
       <c r="J3" s="12" t="s">
@@ -5498,12 +5487,12 @@
         <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="94">
+      <c r="I4" s="93">
         <v>0</v>
       </c>
       <c r="J4" s="12" t="s">
@@ -5530,12 +5519,12 @@
         <v>30</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="94">
+      <c r="I5" s="93">
         <v>0</v>
       </c>
       <c r="J5" s="12" t="s">
@@ -5562,12 +5551,12 @@
         <v>30</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="94">
+      <c r="I6" s="93">
         <v>0</v>
       </c>
       <c r="J6" s="12" t="s">
@@ -5594,12 +5583,12 @@
         <v>30</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="94">
+      <c r="I7" s="93">
         <v>0</v>
       </c>
       <c r="J7" s="12" t="s">
@@ -5626,12 +5615,12 @@
         <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="94">
+      <c r="I8" s="93">
         <v>1</v>
       </c>
       <c r="J8" s="12" t="s">
@@ -5658,12 +5647,12 @@
         <v>30</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="94">
+      <c r="I9" s="93">
         <v>1</v>
       </c>
       <c r="J9" s="12" t="s">
@@ -5690,12 +5679,12 @@
         <v>30</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="94">
+      <c r="I10" s="93">
         <v>1</v>
       </c>
       <c r="J10" s="12" t="s">
@@ -5722,12 +5711,12 @@
         <v>30</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="94">
+      <c r="I11" s="93">
         <v>1</v>
       </c>
       <c r="J11" s="12" t="s">
@@ -5754,12 +5743,12 @@
         <v>30</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="94">
+      <c r="I12" s="93">
         <v>1</v>
       </c>
       <c r="J12" s="12" t="s">
@@ -5786,12 +5775,12 @@
         <v>30</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="94">
+      <c r="I13" s="93">
         <v>1</v>
       </c>
       <c r="J13" s="12" t="s">
@@ -5818,12 +5807,12 @@
         <v>30</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="94">
+      <c r="I14" s="93">
         <v>2</v>
       </c>
       <c r="J14" s="12" t="s">
@@ -5850,12 +5839,12 @@
         <v>30</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="94">
+      <c r="I15" s="93">
         <v>2</v>
       </c>
       <c r="J15" s="12" t="s">
@@ -5882,12 +5871,12 @@
         <v>30</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="94">
+      <c r="I16" s="93">
         <v>2</v>
       </c>
       <c r="J16" s="12" t="s">
@@ -5914,12 +5903,12 @@
         <v>30</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="94">
+      <c r="I17" s="93">
         <v>2</v>
       </c>
       <c r="J17" s="12" t="s">
@@ -5946,12 +5935,12 @@
         <v>30</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I18" s="94">
+      <c r="I18" s="93">
         <v>2</v>
       </c>
       <c r="J18" s="12" t="s">
@@ -5978,12 +5967,12 @@
         <v>30</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="94">
+      <c r="I19" s="93">
         <v>2</v>
       </c>
       <c r="J19" s="12" t="s">
@@ -6010,12 +5999,12 @@
         <v>30</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="94">
+      <c r="I20" s="93">
         <v>3</v>
       </c>
       <c r="J20" s="12" t="s">
@@ -6042,12 +6031,12 @@
         <v>30</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="94">
+      <c r="I21" s="93">
         <v>3</v>
       </c>
       <c r="J21" s="12" t="s">
@@ -6074,12 +6063,12 @@
         <v>30</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="94">
+      <c r="I22" s="93">
         <v>3</v>
       </c>
       <c r="J22" s="12" t="s">
@@ -6106,12 +6095,12 @@
         <v>30</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="94">
+      <c r="I23" s="93">
         <v>3</v>
       </c>
       <c r="J23" s="12" t="s">
@@ -6138,12 +6127,12 @@
         <v>30</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="94">
+      <c r="I24" s="93">
         <v>3</v>
       </c>
       <c r="J24" s="12" t="s">
@@ -6170,12 +6159,12 @@
         <v>30</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I25" s="94">
+      <c r="I25" s="93">
         <v>3</v>
       </c>
       <c r="J25" s="12" t="s">
@@ -6202,12 +6191,12 @@
         <v>30</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I26" s="94">
+      <c r="I26" s="93">
         <v>4</v>
       </c>
       <c r="J26" s="12" t="s">
@@ -6234,12 +6223,12 @@
         <v>30</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I27" s="94">
+      <c r="I27" s="93">
         <v>4</v>
       </c>
       <c r="J27" s="12" t="s">
@@ -6266,12 +6255,12 @@
         <v>30</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="94">
+      <c r="I28" s="93">
         <v>4</v>
       </c>
       <c r="J28" s="12" t="s">
@@ -6298,12 +6287,12 @@
         <v>30</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I29" s="94">
+      <c r="I29" s="93">
         <v>4</v>
       </c>
       <c r="J29" s="12" t="s">
@@ -6330,12 +6319,12 @@
         <v>30</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I30" s="94">
+      <c r="I30" s="93">
         <v>4</v>
       </c>
       <c r="J30" s="12" t="s">
@@ -6362,12 +6351,12 @@
         <v>30</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I31" s="94">
+      <c r="I31" s="93">
         <v>4</v>
       </c>
       <c r="J31" s="12" t="s">
@@ -6394,12 +6383,12 @@
         <v>30</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="94">
+      <c r="I32" s="93">
         <v>4</v>
       </c>
       <c r="J32" s="12" t="s">
@@ -6426,12 +6415,12 @@
         <v>30</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I33" s="94">
+      <c r="I33" s="93">
         <v>4</v>
       </c>
       <c r="J33" s="12" t="s">

</xml_diff>

<commit_message>
Update baseurl in config file. Update the functions for country and title drop downs
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="8970" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="8970" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -1374,12 +1374,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1601,27 +1608,27 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1630,7 +1637,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1642,17 +1649,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1661,7 +1668,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1676,26 +1683,26 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1707,10 +1714,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1725,16 +1732,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1744,7 +1751,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1756,7 +1763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1765,18 +1772,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1785,82 +1792,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="15" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="15" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2241,8 +2248,8 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3685,8 +3692,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3740,8 +3747,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3804,8 +3811,8 @@
       <c r="D2" s="71" t="s">
         <v>354</v>
       </c>
-      <c r="E2" s="95" t="s">
-        <v>96</v>
+      <c r="E2" s="96" t="s">
+        <v>25</v>
       </c>
       <c r="F2" s="89" t="s">
         <v>349</v>
@@ -3830,8 +3837,8 @@
       <c r="D3" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="95" t="s">
-        <v>101</v>
+      <c r="E3" s="96" t="s">
+        <v>27</v>
       </c>
       <c r="F3" s="71" t="s">
         <v>356</v>
@@ -3850,14 +3857,14 @@
       <c r="B4" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="95" t="s">
         <v>436</v>
       </c>
       <c r="D4" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="95" t="s">
-        <v>105</v>
+      <c r="E4" s="96" t="s">
+        <v>28</v>
       </c>
       <c r="F4" s="71" t="s">
         <v>356</v>
@@ -3884,8 +3891,8 @@
       <c r="D5" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="95" t="s">
-        <v>109</v>
+      <c r="E5" s="96" t="s">
+        <v>29</v>
       </c>
       <c r="F5" s="71"/>
       <c r="G5" s="71" t="s">
@@ -3912,8 +3919,8 @@
       <c r="D6" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="95" t="s">
-        <v>52</v>
+      <c r="E6" s="96" t="s">
+        <v>30</v>
       </c>
       <c r="F6" s="71" t="s">
         <v>356</v>
@@ -3940,8 +3947,8 @@
       <c r="D7" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="95" t="s">
-        <v>53</v>
+      <c r="E7" s="96" t="s">
+        <v>31</v>
       </c>
       <c r="F7" s="71"/>
       <c r="G7" s="71"/>
@@ -4391,7 +4398,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5302,7 +5309,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
* Update dev url * Update registration function
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="8970" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="8970" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="439">
   <si>
     <t>Browser</t>
   </si>
@@ -824,31 +824,13 @@
     <t>0599226323</t>
   </si>
   <si>
-    <t>companyName</t>
-  </si>
-  <si>
     <t>adddressLine2</t>
   </si>
   <si>
-    <t>position</t>
-  </si>
-  <si>
-    <t>extension</t>
-  </si>
-  <si>
-    <t>QA Lead</t>
-  </si>
-  <si>
     <t>5555555555</t>
   </si>
   <si>
     <t>Mr</t>
-  </si>
-  <si>
-    <t>Callawaygolf</t>
-  </si>
-  <si>
-    <t>QA Tester</t>
   </si>
   <si>
     <t>ThankyouValidation:User registered with success.</t>
@@ -1369,17 +1351,48 @@
   <si>
     <t>update Personal Details</t>
   </si>
+  <si>
+    <t>accountName</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>accountNumber</t>
+  </si>
+  <si>
+    <t>343</t>
+  </si>
+  <si>
+    <t>enteredBy</t>
+  </si>
+  <si>
+    <t>Auto QA</t>
+  </si>
+  <si>
+    <t>QA Auto Test</t>
+  </si>
+  <si>
+    <t>QA Lead</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1608,27 +1621,27 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1637,7 +1650,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1649,17 +1662,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1668,7 +1681,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1683,26 +1696,26 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1714,10 +1727,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1732,16 +1745,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1751,7 +1764,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1763,27 +1776,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1792,82 +1804,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2205,7 +2218,7 @@
       <c r="A2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="59" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2298,16 +2311,16 @@
         <v>179</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F2" s="59" t="s">
-        <v>270</v>
+      <c r="F2" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G2" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2321,16 +2334,16 @@
         <v>179</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F3" s="59" t="s">
-        <v>270</v>
+      <c r="F3" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G3" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2344,16 +2357,16 @@
         <v>179</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F4" s="59" t="s">
-        <v>270</v>
+      <c r="F4" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2367,16 +2380,16 @@
         <v>179</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F5" s="59" t="s">
-        <v>270</v>
+      <c r="F5" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2390,16 +2403,16 @@
         <v>179</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F6" s="59" t="s">
-        <v>270</v>
+      <c r="F6" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2413,16 +2426,16 @@
         <v>179</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="58" t="s">
+        <v>264</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>270</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2436,16 +2449,16 @@
         <v>179</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F8" s="59" t="s">
-        <v>270</v>
+      <c r="F8" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2459,16 +2472,16 @@
         <v>179</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F9" s="59" t="s">
-        <v>270</v>
+      <c r="F9" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2482,16 +2495,16 @@
         <v>179</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F10" s="59" t="s">
-        <v>270</v>
+      <c r="F10" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -2505,16 +2518,16 @@
         <v>179</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F11" s="59" t="s">
-        <v>270</v>
+      <c r="F11" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2528,16 +2541,16 @@
         <v>179</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F12" s="59" t="s">
-        <v>270</v>
+      <c r="F12" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2551,16 +2564,16 @@
         <v>179</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F13" s="59" t="s">
-        <v>270</v>
+      <c r="F13" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2574,16 +2587,16 @@
         <v>179</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F14" s="59" t="s">
-        <v>270</v>
+      <c r="F14" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2597,16 +2610,16 @@
         <v>179</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F15" s="59" t="s">
-        <v>270</v>
+      <c r="F15" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2620,16 +2633,16 @@
         <v>179</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F16" s="59" t="s">
-        <v>270</v>
+      <c r="F16" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2643,16 +2656,16 @@
         <v>179</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F17" s="59" t="s">
-        <v>270</v>
+      <c r="F17" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2666,16 +2679,16 @@
         <v>179</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F18" s="59" t="s">
-        <v>270</v>
+      <c r="F18" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2689,16 +2702,16 @@
         <v>179</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F19" s="59" t="s">
-        <v>270</v>
+      <c r="F19" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2712,16 +2725,16 @@
         <v>179</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F20" s="59" t="s">
-        <v>270</v>
+      <c r="F20" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2735,16 +2748,16 @@
         <v>179</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F21" s="59" t="s">
-        <v>270</v>
+      <c r="F21" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2758,16 +2771,16 @@
         <v>179</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F22" s="59" t="s">
-        <v>270</v>
+      <c r="F22" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2781,16 +2794,16 @@
         <v>179</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="F23" s="59" t="s">
-        <v>270</v>
-      </c>
-      <c r="G23" s="58" t="s">
-        <v>292</v>
+      <c r="F23" s="58" t="s">
+        <v>264</v>
+      </c>
+      <c r="G23" s="57" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2804,16 +2817,16 @@
         <v>179</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F24" s="59" t="s">
-        <v>270</v>
+      <c r="F24" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2827,16 +2840,16 @@
         <v>179</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F25" s="59" t="s">
-        <v>270</v>
+      <c r="F25" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2850,16 +2863,16 @@
         <v>179</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F26" s="59" t="s">
-        <v>270</v>
+      <c r="F26" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2873,16 +2886,16 @@
         <v>179</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F27" s="59" t="s">
-        <v>270</v>
+      <c r="F27" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2896,16 +2909,16 @@
         <v>179</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F28" s="59" t="s">
-        <v>270</v>
+      <c r="F28" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2919,16 +2932,16 @@
         <v>179</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F29" s="59" t="s">
-        <v>270</v>
+      <c r="F29" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2942,16 +2955,16 @@
         <v>179</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F30" s="59" t="s">
-        <v>270</v>
+      <c r="F30" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2965,16 +2978,16 @@
         <v>179</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F31" s="59" t="s">
-        <v>270</v>
+      <c r="F31" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2988,16 +3001,16 @@
         <v>179</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F32" s="59" t="s">
-        <v>270</v>
+      <c r="F32" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -3011,21 +3024,21 @@
         <v>179</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F33" s="59" t="s">
-        <v>270</v>
+      <c r="F33" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="12" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>178</v>
@@ -3034,16 +3047,16 @@
         <v>179</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F34" s="59" t="s">
-        <v>270</v>
+      <c r="F34" s="58" t="s">
+        <v>264</v>
       </c>
       <c r="G34" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -3248,10 +3261,10 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3264,18 +3277,19 @@
     <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="43" t="s">
         <v>215</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C1" s="43" t="s">
         <v>173</v>
@@ -3284,31 +3298,34 @@
         <v>174</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>258</v>
+        <v>431</v>
       </c>
       <c r="F1" s="43" t="s">
         <v>216</v>
       </c>
       <c r="G1" s="43" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H1" s="43" t="s">
         <v>217</v>
       </c>
       <c r="I1" s="43" t="s">
+        <v>432</v>
+      </c>
+      <c r="J1" s="43" t="s">
         <v>218</v>
       </c>
-      <c r="J1" s="43" t="s">
-        <v>260</v>
-      </c>
       <c r="K1" s="43" t="s">
+        <v>433</v>
+      </c>
+      <c r="L1" s="43" t="s">
         <v>219</v>
       </c>
-      <c r="L1" s="43" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="43" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
         <v>220</v>
       </c>
@@ -3316,13 +3333,13 @@
         <v>231</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>266</v>
+        <v>438</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>265</v>
+        <v>437</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>228</v>
@@ -3332,17 +3349,22 @@
         <v>229</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="L2" s="57"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="K2" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="M2" s="96" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>225</v>
       </c>
@@ -3353,10 +3375,10 @@
         <v>178</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>266</v>
+        <v>438</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>265</v>
+        <v>437</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>226</v>
@@ -3365,18 +3387,19 @@
       <c r="H3" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="5"/>
+      <c r="J3" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="L3" s="57"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="K3" s="5"/>
+      <c r="L3" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="M3" s="96" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -3387,10 +3410,10 @@
         <v>178</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>266</v>
+        <v>438</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>265</v>
+        <v>437</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>221</v>
@@ -3399,18 +3422,19 @@
       <c r="H4" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="L4" s="57"/>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="K4" s="5"/>
+      <c r="L4" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="M4" s="96" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
         <v>232</v>
       </c>
@@ -3421,10 +3445,10 @@
         <v>178</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>266</v>
+        <v>438</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>265</v>
+        <v>437</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>233</v>
@@ -3433,88 +3457,91 @@
       <c r="H5" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="L5" s="57"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="K5" s="5"/>
+      <c r="L5" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="M5" s="96" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="B6" s="64" t="s">
-        <v>336</v>
+        <v>331</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>330</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>178</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>266</v>
+        <v>438</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>265</v>
+        <v>437</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="I6" s="4">
+        <v>333</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4">
         <v>5526</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="K6" s="5"/>
+      <c r="L6" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="M6" s="96" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="B7" s="64" t="s">
-        <v>418</v>
-      </c>
-      <c r="C7" s="92" t="s">
-        <v>419</v>
+        <v>411</v>
+      </c>
+      <c r="B7" s="63" t="s">
+        <v>412</v>
+      </c>
+      <c r="C7" s="91" t="s">
+        <v>413</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>266</v>
+        <v>438</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>265</v>
+        <v>437</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>421</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="L7" s="4"/>
+        <v>415</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="M7" s="96" t="s">
+        <v>436</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3728,7 +3755,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B4" s="52" t="s">
         <v>7</v>
@@ -3747,219 +3774,219 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="69" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="69" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="69" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="74" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="69" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" style="69" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="69"/>
+    <col min="1" max="1" width="6.5703125" style="68" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="68" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="68" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="68" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="68" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" style="68" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="68"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="66" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="67" t="s">
+        <v>344</v>
+      </c>
+      <c r="G1" s="67" t="s">
+        <v>176</v>
+      </c>
+      <c r="H1" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="67" t="s">
+        <v>345</v>
+      </c>
+      <c r="J1" s="67" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="89" t="s">
+        <v>405</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="70" t="s">
+        <v>347</v>
+      </c>
+      <c r="D2" s="70" t="s">
+        <v>348</v>
+      </c>
+      <c r="E2" s="95" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="88" t="s">
+        <v>343</v>
+      </c>
+      <c r="G2" s="70" t="s">
+        <v>180</v>
+      </c>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="89" t="s">
+        <v>406</v>
+      </c>
+      <c r="B3" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="70" t="s">
+        <v>349</v>
+      </c>
+      <c r="D3" s="70" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="95" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="70" t="s">
         <v>350</v>
       </c>
-      <c r="G1" s="68" t="s">
-        <v>176</v>
-      </c>
-      <c r="H1" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="68" t="s">
+      <c r="G3" s="70" t="s">
         <v>351</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+    </row>
+    <row r="4" spans="1:10" ht="30">
+      <c r="A4" s="89" t="s">
+        <v>407</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="94" t="s">
+        <v>430</v>
+      </c>
+      <c r="D4" s="70" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="95" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="70" t="s">
+        <v>350</v>
+      </c>
+      <c r="G4" s="70" t="s">
+        <v>351</v>
+      </c>
+      <c r="H4" s="72" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="90" t="s">
-        <v>411</v>
-      </c>
-      <c r="B2" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="71" t="s">
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+    </row>
+    <row r="5" spans="1:10" ht="30">
+      <c r="A5" s="89" t="s">
+        <v>408</v>
+      </c>
+      <c r="B5" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="70" t="s">
         <v>353</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="D5" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="95" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70" t="s">
+        <v>351</v>
+      </c>
+      <c r="H5" s="72" t="s">
         <v>354</v>
       </c>
-      <c r="E2" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="89" t="s">
-        <v>349</v>
-      </c>
-      <c r="G2" s="71" t="s">
-        <v>180</v>
-      </c>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="90" t="s">
-        <v>412</v>
-      </c>
-      <c r="B3" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="71" t="s">
+      <c r="I5" s="71" t="s">
         <v>355</v>
       </c>
-      <c r="D3" s="71" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="96" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="71" t="s">
+      <c r="J5" s="71"/>
+    </row>
+    <row r="6" spans="1:10" ht="30">
+      <c r="A6" s="89" t="s">
+        <v>409</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="70" t="s">
         <v>356</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="D6" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="95" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="70" t="s">
+        <v>350</v>
+      </c>
+      <c r="G6" s="70"/>
+      <c r="H6" s="72" t="s">
+        <v>354</v>
+      </c>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71" t="s">
         <v>357</v>
       </c>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-    </row>
-    <row r="4" spans="1:10" ht="30">
-      <c r="A4" s="90" t="s">
-        <v>413</v>
-      </c>
-      <c r="B4" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="95" t="s">
-        <v>436</v>
-      </c>
-      <c r="D4" s="71" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" s="96" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="71" t="s">
-        <v>356</v>
-      </c>
-      <c r="G4" s="71" t="s">
+    </row>
+    <row r="7" spans="1:10" ht="30">
+      <c r="A7" s="89" t="s">
+        <v>410</v>
+      </c>
+      <c r="B7" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>358</v>
+      </c>
+      <c r="D7" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="95" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="72" t="s">
+        <v>354</v>
+      </c>
+      <c r="I7" s="71" t="s">
+        <v>355</v>
+      </c>
+      <c r="J7" s="71" t="s">
         <v>357</v>
-      </c>
-      <c r="H4" s="73" t="s">
-        <v>358</v>
-      </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-    </row>
-    <row r="5" spans="1:10" ht="30">
-      <c r="A5" s="90" t="s">
-        <v>414</v>
-      </c>
-      <c r="B5" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="71" t="s">
-        <v>359</v>
-      </c>
-      <c r="D5" s="71" t="s">
-        <v>115</v>
-      </c>
-      <c r="E5" s="96" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71" t="s">
-        <v>357</v>
-      </c>
-      <c r="H5" s="73" t="s">
-        <v>360</v>
-      </c>
-      <c r="I5" s="72" t="s">
-        <v>361</v>
-      </c>
-      <c r="J5" s="72"/>
-    </row>
-    <row r="6" spans="1:10" ht="30">
-      <c r="A6" s="90" t="s">
-        <v>415</v>
-      </c>
-      <c r="B6" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="71" t="s">
-        <v>362</v>
-      </c>
-      <c r="D6" s="71" t="s">
-        <v>115</v>
-      </c>
-      <c r="E6" s="96" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="71" t="s">
-        <v>356</v>
-      </c>
-      <c r="G6" s="71"/>
-      <c r="H6" s="73" t="s">
-        <v>360</v>
-      </c>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="30">
-      <c r="A7" s="90" t="s">
-        <v>416</v>
-      </c>
-      <c r="B7" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="71" t="s">
-        <v>364</v>
-      </c>
-      <c r="D7" s="71" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="96" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="73" t="s">
-        <v>360</v>
-      </c>
-      <c r="I7" s="72" t="s">
-        <v>361</v>
-      </c>
-      <c r="J7" s="72" t="s">
-        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -3980,409 +4007,409 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="69" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="69" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="69" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="76" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="75" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" style="75" customWidth="1"/>
-    <col min="8" max="8" width="10" style="75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" style="75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" style="75" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="24.7109375" style="75" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="69"/>
+    <col min="1" max="1" width="8.42578125" style="68" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="68" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="68" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" style="74" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" style="74" customWidth="1"/>
+    <col min="8" max="8" width="10" style="74" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="24.7109375" style="74" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="68"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="88" t="s">
+      <c r="D1" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="88" t="s">
+      <c r="E1" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="88" t="s">
-        <v>410</v>
-      </c>
-      <c r="G1" s="88" t="s">
-        <v>409</v>
-      </c>
-      <c r="H1" s="88" t="s">
+      <c r="F1" s="87" t="s">
+        <v>404</v>
+      </c>
+      <c r="G1" s="87" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="87" t="s">
+      <c r="I1" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="86" t="s">
-        <v>408</v>
-      </c>
-      <c r="K1" s="85" t="s">
-        <v>407</v>
-      </c>
-      <c r="L1" s="85" t="s">
-        <v>406</v>
+      <c r="J1" s="85" t="s">
+        <v>402</v>
+      </c>
+      <c r="K1" s="84" t="s">
+        <v>401</v>
+      </c>
+      <c r="L1" s="84" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="81" t="s">
-        <v>405</v>
-      </c>
-      <c r="B2" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="79" t="s">
-        <v>404</v>
-      </c>
-      <c r="D2" s="91" t="s">
+      <c r="A2" s="80" t="s">
+        <v>399</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="78" t="s">
+        <v>398</v>
+      </c>
+      <c r="D2" s="90" t="s">
+        <v>348</v>
+      </c>
+      <c r="E2" s="93" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="80" t="s">
+        <v>397</v>
+      </c>
+      <c r="B3" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="78" t="s">
+        <v>396</v>
+      </c>
+      <c r="D3" s="70" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="93" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="83" t="s">
+        <v>395</v>
+      </c>
+      <c r="G3" s="83" t="s">
+        <v>395</v>
+      </c>
+      <c r="H3" s="78">
+        <v>1234567</v>
+      </c>
+      <c r="I3" s="77"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+    </row>
+    <row r="4" spans="1:12" ht="30">
+      <c r="A4" s="80" t="s">
+        <v>394</v>
+      </c>
+      <c r="B4" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="78" t="s">
+        <v>393</v>
+      </c>
+      <c r="D4" s="70" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="93" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="81" t="s">
+        <v>392</v>
+      </c>
+      <c r="G4" s="81" t="s">
+        <v>392</v>
+      </c>
+      <c r="H4" s="78">
+        <v>1234567</v>
+      </c>
+      <c r="I4" s="77" t="s">
+        <v>352</v>
+      </c>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="80" t="s">
+        <v>391</v>
+      </c>
+      <c r="B5" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="78" t="s">
+        <v>390</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="93" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="70"/>
+      <c r="G5" s="79" t="s">
+        <v>389</v>
+      </c>
+      <c r="H5" s="78">
+        <v>1234567</v>
+      </c>
+      <c r="I5" s="77" t="s">
         <v>354</v>
       </c>
-      <c r="E2" s="94" t="s">
+      <c r="J5" s="77" t="s">
+        <v>314</v>
+      </c>
+      <c r="K5" s="77"/>
+      <c r="L5" s="76"/>
+    </row>
+    <row r="6" spans="1:12" ht="30">
+      <c r="A6" s="80" t="s">
+        <v>388</v>
+      </c>
+      <c r="B6" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="78" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="93" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="81" t="s">
+        <v>386</v>
+      </c>
+      <c r="G6" s="70"/>
+      <c r="H6" s="78">
+        <v>1234567</v>
+      </c>
+      <c r="I6" s="77" t="s">
+        <v>354</v>
+      </c>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77" t="s">
+        <v>385</v>
+      </c>
+      <c r="L6" s="76"/>
+    </row>
+    <row r="7" spans="1:12" ht="30">
+      <c r="A7" s="80" t="s">
+        <v>384</v>
+      </c>
+      <c r="B7" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="78" t="s">
+        <v>383</v>
+      </c>
+      <c r="D7" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="93" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="79" t="s">
+        <v>382</v>
+      </c>
+      <c r="G7" s="79" t="s">
+        <v>382</v>
+      </c>
+      <c r="H7" s="78"/>
+      <c r="I7" s="77" t="s">
+        <v>354</v>
+      </c>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="76" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="80" t="s">
+        <v>380</v>
+      </c>
+      <c r="B8" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="78" t="s">
+        <v>379</v>
+      </c>
+      <c r="D8" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="93" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="70" t="s">
+        <v>378</v>
+      </c>
+      <c r="G8" s="79" t="s">
+        <v>377</v>
+      </c>
+      <c r="H8" s="78">
+        <v>1234567</v>
+      </c>
+      <c r="I8" s="77" t="s">
+        <v>354</v>
+      </c>
+      <c r="J8" s="68" t="s">
+        <v>314</v>
+      </c>
+      <c r="K8" s="77"/>
+      <c r="L8" s="76"/>
+    </row>
+    <row r="9" spans="1:12" ht="30">
+      <c r="A9" s="80" t="s">
+        <v>376</v>
+      </c>
+      <c r="B9" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="78" t="s">
+        <v>375</v>
+      </c>
+      <c r="D9" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="81" t="s">
-        <v>403</v>
-      </c>
-      <c r="B3" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="79" t="s">
-        <v>402</v>
-      </c>
-      <c r="D3" s="71" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="94" t="s">
+      <c r="F9" s="79" t="s">
+        <v>374</v>
+      </c>
+      <c r="G9" s="70" t="s">
+        <v>373</v>
+      </c>
+      <c r="H9" s="78">
+        <v>1234567</v>
+      </c>
+      <c r="I9" s="77" t="s">
+        <v>354</v>
+      </c>
+      <c r="J9" s="77"/>
+      <c r="K9" s="77" t="s">
+        <v>368</v>
+      </c>
+      <c r="L9" s="76"/>
+    </row>
+    <row r="10" spans="1:12" ht="30">
+      <c r="A10" s="80" t="s">
+        <v>372</v>
+      </c>
+      <c r="B10" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="78" t="s">
+        <v>371</v>
+      </c>
+      <c r="D10" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="84" t="s">
-        <v>401</v>
-      </c>
-      <c r="G3" s="84" t="s">
-        <v>401</v>
-      </c>
-      <c r="H3" s="79">
+      <c r="F10" s="79" t="s">
+        <v>370</v>
+      </c>
+      <c r="G10" s="79" t="s">
+        <v>369</v>
+      </c>
+      <c r="H10" s="78">
         <v>1234567</v>
       </c>
-      <c r="I3" s="78"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-    </row>
-    <row r="4" spans="1:12" ht="30">
-      <c r="A4" s="81" t="s">
-        <v>400</v>
-      </c>
-      <c r="B4" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="79" t="s">
-        <v>399</v>
-      </c>
-      <c r="D4" s="71" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" s="94" t="s">
+      <c r="I10" s="77" t="s">
+        <v>354</v>
+      </c>
+      <c r="J10" s="77"/>
+      <c r="K10" s="77" t="s">
+        <v>368</v>
+      </c>
+      <c r="L10" s="76"/>
+    </row>
+    <row r="11" spans="1:12" ht="30">
+      <c r="A11" s="80" t="s">
+        <v>367</v>
+      </c>
+      <c r="B11" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="78" t="s">
+        <v>366</v>
+      </c>
+      <c r="D11" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="93" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="82" t="s">
-        <v>398</v>
-      </c>
-      <c r="G4" s="82" t="s">
-        <v>398</v>
-      </c>
-      <c r="H4" s="79">
+      <c r="F11" s="79" t="s">
+        <v>365</v>
+      </c>
+      <c r="G11" s="79" t="s">
+        <v>365</v>
+      </c>
+      <c r="H11" s="78">
+        <v>874531324</v>
+      </c>
+      <c r="I11" s="77" t="s">
+        <v>354</v>
+      </c>
+      <c r="J11" s="77"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="76" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30">
+      <c r="A12" s="80" t="s">
+        <v>363</v>
+      </c>
+      <c r="B12" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="78" t="s">
+        <v>362</v>
+      </c>
+      <c r="D12" s="70" t="s">
+        <v>361</v>
+      </c>
+      <c r="E12" s="93" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="79" t="s">
+        <v>360</v>
+      </c>
+      <c r="G12" s="79" t="s">
+        <v>360</v>
+      </c>
+      <c r="H12" s="78">
         <v>1234567</v>
       </c>
-      <c r="I4" s="78" t="s">
-        <v>358</v>
-      </c>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="81" t="s">
-        <v>397</v>
-      </c>
-      <c r="B5" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="79" t="s">
-        <v>396</v>
-      </c>
-      <c r="D5" s="71" t="s">
-        <v>115</v>
-      </c>
-      <c r="E5" s="94" t="s">
-        <v>143</v>
-      </c>
-      <c r="F5" s="71"/>
-      <c r="G5" s="80" t="s">
-        <v>395</v>
-      </c>
-      <c r="H5" s="79">
-        <v>1234567</v>
-      </c>
-      <c r="I5" s="78" t="s">
-        <v>360</v>
-      </c>
-      <c r="J5" s="78" t="s">
-        <v>320</v>
-      </c>
-      <c r="K5" s="78"/>
-      <c r="L5" s="77"/>
-    </row>
-    <row r="6" spans="1:12" ht="30">
-      <c r="A6" s="81" t="s">
-        <v>394</v>
-      </c>
-      <c r="B6" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="79" t="s">
-        <v>393</v>
-      </c>
-      <c r="D6" s="71" t="s">
-        <v>115</v>
-      </c>
-      <c r="E6" s="94" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="82" t="s">
-        <v>392</v>
-      </c>
-      <c r="G6" s="71"/>
-      <c r="H6" s="79">
-        <v>1234567</v>
-      </c>
-      <c r="I6" s="78" t="s">
-        <v>360</v>
-      </c>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78" t="s">
-        <v>391</v>
-      </c>
-      <c r="L6" s="77"/>
-    </row>
-    <row r="7" spans="1:12" ht="30">
-      <c r="A7" s="81" t="s">
-        <v>390</v>
-      </c>
-      <c r="B7" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="79" t="s">
-        <v>389</v>
-      </c>
-      <c r="D7" s="71" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="94" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="80" t="s">
-        <v>388</v>
-      </c>
-      <c r="G7" s="80" t="s">
-        <v>388</v>
-      </c>
-      <c r="H7" s="79"/>
-      <c r="I7" s="78" t="s">
-        <v>360</v>
-      </c>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="77" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="81" t="s">
-        <v>386</v>
-      </c>
-      <c r="B8" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="79" t="s">
-        <v>385</v>
-      </c>
-      <c r="D8" s="71" t="s">
-        <v>115</v>
-      </c>
-      <c r="E8" s="94" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="71" t="s">
-        <v>384</v>
-      </c>
-      <c r="G8" s="80" t="s">
-        <v>383</v>
-      </c>
-      <c r="H8" s="79">
-        <v>1234567</v>
-      </c>
-      <c r="I8" s="78" t="s">
-        <v>360</v>
-      </c>
-      <c r="J8" s="69" t="s">
-        <v>320</v>
-      </c>
-      <c r="K8" s="78"/>
-      <c r="L8" s="77"/>
-    </row>
-    <row r="9" spans="1:12" ht="30">
-      <c r="A9" s="81" t="s">
-        <v>382</v>
-      </c>
-      <c r="B9" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="79" t="s">
-        <v>381</v>
-      </c>
-      <c r="D9" s="71" t="s">
-        <v>115</v>
-      </c>
-      <c r="E9" s="94" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="80" t="s">
-        <v>380</v>
-      </c>
-      <c r="G9" s="71" t="s">
-        <v>379</v>
-      </c>
-      <c r="H9" s="79">
-        <v>1234567</v>
-      </c>
-      <c r="I9" s="78" t="s">
-        <v>360</v>
-      </c>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78" t="s">
-        <v>374</v>
-      </c>
-      <c r="L9" s="77"/>
-    </row>
-    <row r="10" spans="1:12" ht="30">
-      <c r="A10" s="81" t="s">
-        <v>378</v>
-      </c>
-      <c r="B10" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="79" t="s">
-        <v>377</v>
-      </c>
-      <c r="D10" s="71" t="s">
-        <v>115</v>
-      </c>
-      <c r="E10" s="94" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="80" t="s">
-        <v>376</v>
-      </c>
-      <c r="G10" s="80" t="s">
-        <v>375</v>
-      </c>
-      <c r="H10" s="79">
-        <v>1234567</v>
-      </c>
-      <c r="I10" s="78" t="s">
-        <v>360</v>
-      </c>
-      <c r="J10" s="78"/>
-      <c r="K10" s="78" t="s">
-        <v>374</v>
-      </c>
-      <c r="L10" s="77"/>
-    </row>
-    <row r="11" spans="1:12" ht="30">
-      <c r="A11" s="81" t="s">
-        <v>373</v>
-      </c>
-      <c r="B11" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="79" t="s">
-        <v>372</v>
-      </c>
-      <c r="D11" s="71" t="s">
-        <v>115</v>
-      </c>
-      <c r="E11" s="94" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="80" t="s">
-        <v>371</v>
-      </c>
-      <c r="G11" s="80" t="s">
-        <v>371</v>
-      </c>
-      <c r="H11" s="79">
-        <v>874531324</v>
-      </c>
-      <c r="I11" s="78" t="s">
-        <v>360</v>
-      </c>
-      <c r="J11" s="78"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="77" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="30">
-      <c r="A12" s="81" t="s">
-        <v>369</v>
-      </c>
-      <c r="B12" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="79" t="s">
-        <v>368</v>
-      </c>
-      <c r="D12" s="71" t="s">
-        <v>367</v>
-      </c>
-      <c r="E12" s="94" t="s">
-        <v>143</v>
-      </c>
-      <c r="F12" s="80" t="s">
-        <v>366</v>
-      </c>
-      <c r="G12" s="80" t="s">
-        <v>366</v>
-      </c>
-      <c r="H12" s="79">
-        <v>1234567</v>
-      </c>
-      <c r="I12" s="78" t="s">
-        <v>360</v>
-      </c>
-      <c r="J12" s="78" t="s">
-        <v>365</v>
-      </c>
-      <c r="K12" s="78"/>
-      <c r="L12" s="77"/>
+      <c r="I12" s="77" t="s">
+        <v>354</v>
+      </c>
+      <c r="J12" s="77" t="s">
+        <v>359</v>
+      </c>
+      <c r="K12" s="77"/>
+      <c r="L12" s="76"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4441,7 +4468,7 @@
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>7</v>
@@ -4465,7 +4492,7 @@
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>7</v>
@@ -4491,7 +4518,7 @@
     </row>
     <row r="4" spans="1:8" ht="30">
       <c r="A4" s="34" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>7</v>
@@ -4517,7 +4544,7 @@
     </row>
     <row r="5" spans="1:8" ht="60">
       <c r="A5" s="34" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>7</v>
@@ -4543,7 +4570,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="34" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>7</v>
@@ -4562,12 +4589,12 @@
         <v>102</v>
       </c>
       <c r="H6" s="38" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
       <c r="A7" s="34" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>7</v>
@@ -4593,7 +4620,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="34" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>7</v>
@@ -4612,12 +4639,12 @@
       </c>
       <c r="G8" s="34"/>
       <c r="H8" s="38" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
       <c r="A9" s="34" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>7</v>
@@ -4643,7 +4670,7 @@
     </row>
     <row r="10" spans="1:8" ht="30">
       <c r="A10" s="34" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>7</v>
@@ -4669,7 +4696,7 @@
     </row>
     <row r="11" spans="1:8" ht="30">
       <c r="A11" s="34" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>7</v>
@@ -4739,155 +4766,155 @@
       <c r="A2" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="64"/>
       <c r="C2" s="53" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D2" s="53" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="53" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45">
       <c r="A3" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="65"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="53" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="E3" s="53" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45">
       <c r="A4" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="65"/>
+      <c r="B4" s="64"/>
       <c r="C4" s="53" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D4" s="53" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45">
       <c r="A5" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="65"/>
+      <c r="B5" s="64"/>
       <c r="C5" s="53" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D5" s="53" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45">
       <c r="A6" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="64" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D6" s="53" t="s">
         <v>42</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45">
       <c r="A7" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="64" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="53" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D7" s="53" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45">
       <c r="A8" s="53" t="s">
-        <v>317</v>
-      </c>
-      <c r="B8" s="65" t="s">
+        <v>311</v>
+      </c>
+      <c r="B8" s="64" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D8" s="53" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45">
       <c r="A9" s="53" t="s">
-        <v>318</v>
-      </c>
-      <c r="B9" s="65"/>
+        <v>312</v>
+      </c>
+      <c r="B9" s="64"/>
       <c r="C9" s="53" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D9" s="53" t="s">
         <v>46</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="53" t="s">
-        <v>345</v>
-      </c>
-      <c r="B10" s="65" t="s">
+        <v>339</v>
+      </c>
+      <c r="B10" s="64" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D10" s="53" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="E10" s="53"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="53" t="s">
-        <v>346</v>
-      </c>
-      <c r="B11" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="66" t="s">
-        <v>343</v>
-      </c>
-      <c r="D11" s="66" t="s">
-        <v>348</v>
+        <v>340</v>
+      </c>
+      <c r="B11" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>337</v>
+      </c>
+      <c r="D11" s="65" t="s">
+        <v>342</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -4903,8 +4930,8 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D2:D6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4947,24 +4974,22 @@
         <v>63</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="39" customFormat="1">
       <c r="A3" s="47" t="s">
-        <v>341</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>7</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="B3" s="12"/>
       <c r="C3" s="48" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4981,7 +5006,7 @@
         <v>66</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="150">
@@ -4997,8 +5022,8 @@
       <c r="D5" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="61" t="s">
-        <v>271</v>
+      <c r="E5" s="60" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -5015,7 +5040,7 @@
         <v>72</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -5178,7 +5203,7 @@
         <v>25</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5196,101 +5221,101 @@
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="44" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="22" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="44"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="22" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="44"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="22" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="62" t="s">
-        <v>327</v>
+      <c r="C11" s="61" t="s">
+        <v>321</v>
       </c>
       <c r="D11" s="44" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="44"/>
     </row>
     <row r="12" spans="1:6" ht="30">
       <c r="A12" s="22" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="41"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="22" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="63" t="s">
-        <v>328</v>
+      <c r="C13" s="62" t="s">
+        <v>322</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="22" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="63" t="s">
-        <v>329</v>
-      </c>
-      <c r="D14" s="63" t="s">
-        <v>329</v>
+      <c r="C14" s="62" t="s">
+        <v>323</v>
+      </c>
+      <c r="D14" s="62" t="s">
+        <v>323</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -5309,7 +5334,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5352,7 +5377,7 @@
         <v>18</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>19</v>
@@ -5378,7 +5403,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>22</v>
@@ -5410,12 +5435,12 @@
         <v>24</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="93">
+      <c r="I3" s="92">
         <v>0</v>
       </c>
       <c r="J3" s="12" t="s">
@@ -5442,12 +5467,12 @@
         <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="93">
+      <c r="I4" s="92">
         <v>0</v>
       </c>
       <c r="J4" s="12" t="s">
@@ -5474,12 +5499,12 @@
         <v>24</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="93">
+      <c r="I5" s="92">
         <v>0</v>
       </c>
       <c r="J5" s="12" t="s">
@@ -5506,12 +5531,12 @@
         <v>24</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="93">
+      <c r="I6" s="92">
         <v>0</v>
       </c>
       <c r="J6" s="12" t="s">
@@ -5538,12 +5563,12 @@
         <v>24</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="93">
+      <c r="I7" s="92">
         <v>0</v>
       </c>
       <c r="J7" s="12" t="s">
@@ -5570,12 +5595,12 @@
         <v>24</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="93">
+      <c r="I8" s="92">
         <v>1</v>
       </c>
       <c r="J8" s="12" t="s">
@@ -5602,12 +5627,12 @@
         <v>24</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="93">
+      <c r="I9" s="92">
         <v>1</v>
       </c>
       <c r="J9" s="12" t="s">
@@ -5634,12 +5659,12 @@
         <v>24</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="93">
+      <c r="I10" s="92">
         <v>1</v>
       </c>
       <c r="J10" s="12" t="s">
@@ -5666,12 +5691,12 @@
         <v>24</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="93">
+      <c r="I11" s="92">
         <v>1</v>
       </c>
       <c r="J11" s="12" t="s">
@@ -5698,12 +5723,12 @@
         <v>24</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="93">
+      <c r="I12" s="92">
         <v>1</v>
       </c>
       <c r="J12" s="12" t="s">
@@ -5730,12 +5755,12 @@
         <v>24</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="93">
+      <c r="I13" s="92">
         <v>1</v>
       </c>
       <c r="J13" s="12" t="s">
@@ -5762,12 +5787,12 @@
         <v>24</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="93">
+      <c r="I14" s="92">
         <v>2</v>
       </c>
       <c r="J14" s="12" t="s">
@@ -5794,12 +5819,12 @@
         <v>24</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="93">
+      <c r="I15" s="92">
         <v>2</v>
       </c>
       <c r="J15" s="12" t="s">
@@ -5826,12 +5851,12 @@
         <v>24</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="93">
+      <c r="I16" s="92">
         <v>2</v>
       </c>
       <c r="J16" s="12" t="s">
@@ -5858,12 +5883,12 @@
         <v>24</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="93">
+      <c r="I17" s="92">
         <v>2</v>
       </c>
       <c r="J17" s="12" t="s">
@@ -5890,12 +5915,12 @@
         <v>24</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="93">
+      <c r="I18" s="92">
         <v>2</v>
       </c>
       <c r="J18" s="12" t="s">
@@ -5922,12 +5947,12 @@
         <v>24</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="93">
+      <c r="I19" s="92">
         <v>2</v>
       </c>
       <c r="J19" s="12" t="s">
@@ -5954,12 +5979,12 @@
         <v>24</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="93">
+      <c r="I20" s="92">
         <v>3</v>
       </c>
       <c r="J20" s="12" t="s">
@@ -5986,12 +6011,12 @@
         <v>24</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="93">
+      <c r="I21" s="92">
         <v>3</v>
       </c>
       <c r="J21" s="12" t="s">
@@ -6018,12 +6043,12 @@
         <v>24</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I22" s="93">
+      <c r="I22" s="92">
         <v>3</v>
       </c>
       <c r="J22" s="12" t="s">
@@ -6050,12 +6075,12 @@
         <v>24</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="93">
+      <c r="I23" s="92">
         <v>3</v>
       </c>
       <c r="J23" s="12" t="s">
@@ -6082,12 +6107,12 @@
         <v>24</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="93">
+      <c r="I24" s="92">
         <v>3</v>
       </c>
       <c r="J24" s="12" t="s">
@@ -6114,12 +6139,12 @@
         <v>24</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="93">
+      <c r="I25" s="92">
         <v>3</v>
       </c>
       <c r="J25" s="12" t="s">
@@ -6146,12 +6171,12 @@
         <v>24</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="93">
+      <c r="I26" s="92">
         <v>4</v>
       </c>
       <c r="J26" s="12" t="s">
@@ -6178,12 +6203,12 @@
         <v>24</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I27" s="93">
+      <c r="I27" s="92">
         <v>4</v>
       </c>
       <c r="J27" s="12" t="s">
@@ -6210,12 +6235,12 @@
         <v>24</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I28" s="93">
+      <c r="I28" s="92">
         <v>4</v>
       </c>
       <c r="J28" s="12" t="s">
@@ -6242,12 +6267,12 @@
         <v>24</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="93">
+      <c r="I29" s="92">
         <v>4</v>
       </c>
       <c r="J29" s="12" t="s">
@@ -6274,12 +6299,12 @@
         <v>24</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="93">
+      <c r="I30" s="92">
         <v>4</v>
       </c>
       <c r="J30" s="12" t="s">
@@ -6306,12 +6331,12 @@
         <v>24</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I31" s="93">
+      <c r="I31" s="92">
         <v>4</v>
       </c>
       <c r="J31" s="12" t="s">
@@ -6338,12 +6363,12 @@
         <v>24</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="93">
+      <c r="I32" s="92">
         <v>4</v>
       </c>
       <c r="J32" s="12" t="s">
@@ -6370,12 +6395,12 @@
         <v>24</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>417</v>
+        <v>220</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="93">
+      <c r="I33" s="92">
         <v>4</v>
       </c>
       <c r="J33" s="12" t="s">

</xml_diff>